<commit_message>
current script for testing
</commit_message>
<xml_diff>
--- a/working pixel dimensions.xlsx
+++ b/working pixel dimensions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yannick\Desktop\redeem-team-fydp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Documents\GitHub\FYDP\redeem-team-fydp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,7 +386,7 @@
         <v>1440</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C10" si="0">A3*B3</f>
+        <f t="shared" ref="C3:C11" si="0">A3*B3</f>
         <v>2592000</v>
       </c>
     </row>
@@ -481,7 +481,20 @@
         <v>2592000</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2304</v>
+      </c>
+      <c r="B11">
+        <v>1536</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>3538944</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>